<commit_message>
Another set of updates to documetation of etdataset
</commit_message>
<xml_diff>
--- a/source_analyses/eu/2011/0_preparation/list_of_EU_countries.xlsx
+++ b/source_analyses/eu/2011/0_preparation/list_of_EU_countries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
   <si>
     <t>Austria</t>
   </si>
@@ -99,9 +99,6 @@
     <t xml:space="preserve">Sweden </t>
   </si>
   <si>
-    <t>United Kingdom.</t>
-  </si>
-  <si>
     <t>Is there an autoproducer table?</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
   </si>
   <si>
     <t>Turkey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> United Kingdom</t>
   </si>
   <si>
     <r>
@@ -179,7 +173,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">missing countries in OECD Europe autoproducer table: </t>
+    <t xml:space="preserve">Missing countries in OECD Europe autoproducer table: </t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
@@ -234,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -313,6 +310,43 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -342,17 +376,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -703,455 +765,492 @@
   <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="I2" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="12"/>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="15"/>
+      <c r="I6" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="I12" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="2"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="15"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="15"/>
+      <c r="I20" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="F21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="15"/>
+      <c r="I22" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="15"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="2"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="F24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="2"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="F25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="F26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="F27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="F29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="F30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="F31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="F32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="2"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="F33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="2"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="F34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="F2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="I6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="F9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="F10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="F11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="F13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="F15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="F17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="F18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="5"/>
-      <c r="I20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="F21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="B22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="5"/>
-      <c r="I22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="F24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="B26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="F26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="F27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="B28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="5"/>
-      <c r="I28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9">
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="F29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="B30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="F30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="2:9">
-      <c r="B31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="F31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="2:9">
-      <c r="B32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="F32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="F33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="F34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="F35" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="8"/>
+      <c r="C35" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="F35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="I35" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="I2:I3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>